<commit_message>
Revert "Revert "Revert "Revert "观念，情感，行为表--第一版图片版""""
This reverts commit a10228ba409828bebfdeaa07b332f02f052d9a92.
</commit_message>
<xml_diff>
--- a/01读书笔记/《中毒的父母》或者中毒的爱/观念、情感、行为关系表-2021-10-31.xlsx
+++ b/01读书笔记/《中毒的父母》或者中毒的爱/观念、情感、行为关系表-2021-10-31.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19650" windowHeight="7875" activeTab="1"/>
+    <workbookView windowWidth="19650" windowHeight="7920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="观念表" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
   <si>
     <t>添加行说明：可以添加其他行</t>
   </si>
@@ -186,15 +186,16 @@
     <t>当父母试图控制我时,我感到愤怒。</t>
   </si>
   <si>
-    <t>因为如果父母乐于改正,我的自我感觉会好一些。</t>
-  </si>
-  <si>
     <t>当父母告诉我应当怎样生活时,我感到愤怒。</t>
   </si>
   <si>
     <t>当父母告诉我应当怎样思考,应当有什么样的感情或行为时,我感到愤怒。</t>
   </si>
   <si>
+    <t>其实没有必要和父母一直做斗争，做他们的
+对立面，遵从自己的内心，做自己就行。放过自己吧。</t>
+  </si>
+  <si>
     <t>当父母教训我该做什么,不该做什么时,我感到愤怒。</t>
   </si>
   <si>
@@ -208,6 +209,9 @@
   </si>
   <si>
     <t>当父母拒绝我时,我感到愤怒。</t>
+  </si>
+  <si>
+    <t>28/32[很严重哈]</t>
   </si>
   <si>
     <t>顺从型行为:</t>
@@ -271,8 +275,8 @@
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -299,21 +303,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,6 +348,65 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -337,32 +417,17 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -374,73 +439,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -457,37 +461,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,43 +605,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,19 +617,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,67 +635,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,26 +649,47 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -688,31 +713,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -728,17 +738,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -747,157 +751,160 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment vertical="center" wrapText="true"/>
@@ -1362,7 +1369,7 @@
       <c r="B13" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1381,7 +1388,7 @@
       <c r="B15" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1421,17 +1428,18 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="71.375" customWidth="true"/>
-    <col min="3" max="3" width="53.6333333333333" customWidth="true"/>
-    <col min="4" max="4" width="31.25" customWidth="true"/>
+    <col min="2" max="2" width="48.2916666666667" customWidth="true"/>
+    <col min="3" max="3" width="67.7" customWidth="true"/>
+    <col min="4" max="4" width="44.8833333333333" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="true" spans="1:4">
@@ -1571,7 +1579,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1661,9 +1669,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1674,42 +1688,92 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" ht="45" spans="1:4">
+      <c r="A27" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>63</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1725,7 +1789,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1736,7 +1800,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1744,87 +1808,87 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>